<commit_message>
added proximity pair info
</commit_message>
<xml_diff>
--- a/giant anteater info.xlsx
+++ b/giant anteater info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/achhen_student_ubc_ca/Documents/BIOL 452 Directed Studies - Giant Anteaters/Github/giantanteater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{1CCCBD07-EFDE-4D98-B74C-BF46FE785D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A328865-697D-46FF-8FFF-0CC7D1B9C5C3}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{1CCCBD07-EFDE-4D98-B74C-BF46FE785D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B2BB86C-34B2-4024-B809-FF8120078109}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4C6B9C08-2C52-4BF9-A6A3-B1CFF437FEB5}"/>
+    <workbookView xWindow="-17388" yWindow="-2592" windowWidth="17496" windowHeight="30336" xr2:uid="{4C6B9C08-2C52-4BF9-A6A3-B1CFF437FEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +208,33 @@
   </si>
   <si>
     <t>n=4</t>
+  </si>
+  <si>
+    <t>proximity.1.above1</t>
+  </si>
+  <si>
+    <t>anteater_A</t>
+  </si>
+  <si>
+    <t>anteater_B</t>
+  </si>
+  <si>
+    <t>proximity.1.below1</t>
+  </si>
+  <si>
+    <t>proximity.2.above1</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>proximity.2.below1</t>
+  </si>
+  <si>
+    <t>proximity.3.above1</t>
+  </si>
+  <si>
+    <t>proximity.3.below1</t>
   </si>
 </sst>
 </file>
@@ -323,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,6 +386,13 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,23 +713,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FE33E0-F72D-489F-8E43-955E084C8D1D}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
@@ -712,7 +746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -729,7 +763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -746,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -763,7 +797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -777,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -791,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -805,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -819,7 +853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -836,7 +870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -853,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -870,7 +904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -884,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -901,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -910,7 +944,7 @@
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -924,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -941,7 +975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -955,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -963,7 +997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -977,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -994,7 +1028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1008,7 +1042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1025,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1042,7 +1076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1056,7 +1090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1073,7 +1107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1090,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1104,7 +1138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1121,7 +1155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -1138,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1155,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1172,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="13">
         <v>31</v>
       </c>
@@ -1189,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1203,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1217,7 +1251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1231,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1239,7 +1273,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1256,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1273,7 +1307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1290,7 +1324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1304,7 +1338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1312,7 +1346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="13">
         <v>41</v>
       </c>
@@ -1329,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1346,7 +1380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1354,7 +1388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>52</v>
       </c>
@@ -1362,7 +1396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -1379,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -1396,7 +1430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>9</v>
       </c>
@@ -1413,7 +1447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>10</v>
       </c>
@@ -1430,7 +1464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>12</v>
       </c>
@@ -1447,7 +1481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>15</v>
       </c>
@@ -1464,7 +1498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>21</v>
       </c>
@@ -1481,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>24</v>
       </c>
@@ -1498,7 +1532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>27</v>
       </c>
@@ -1515,7 +1549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>29</v>
       </c>
@@ -1532,7 +1566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>36</v>
       </c>
@@ -1549,7 +1583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>38</v>
       </c>
@@ -1566,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
         <v>53</v>
       </c>
@@ -1574,7 +1608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>2</v>
       </c>
@@ -1591,7 +1625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>8</v>
       </c>
@@ -1608,7 +1642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>22</v>
       </c>
@@ -1625,7 +1659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>25</v>
       </c>
@@ -1642,7 +1676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>30</v>
       </c>
@@ -1659,7 +1693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>37</v>
       </c>
@@ -1676,7 +1710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
         <v>42</v>
       </c>
@@ -1693,7 +1727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15" t="s">
         <v>54</v>
       </c>
@@ -1701,7 +1735,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="13">
         <v>19</v>
       </c>
@@ -1718,7 +1752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="13">
         <v>28</v>
       </c>
@@ -1735,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="13">
         <v>31</v>
       </c>
@@ -1752,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="13">
         <v>41</v>
       </c>
@@ -1768,6 +1802,167 @@
       <c r="E76" s="10" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="19"/>
+      <c r="B82" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="19"/>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="19"/>
+      <c r="B85" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="19"/>
+      <c r="B86" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="19"/>
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="19"/>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="19"/>
+      <c r="B89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="19"/>
+      <c r="B91" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="18"/>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="18"/>
+      <c r="B94" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="18"/>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="18"/>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="18"/>
+      <c r="B98" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="18"/>
+      <c r="B100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated individual sex colours
</commit_message>
<xml_diff>
--- a/giant anteater info.xlsx
+++ b/giant anteater info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/achhen_student_ubc_ca/Documents/BIOL 452 Directed Studies - Giant Anteaters/Github/giantanteater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{1CCCBD07-EFDE-4D98-B74C-BF46FE785D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3D6DE6-386F-47A3-A32E-E540EB377361}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{1CCCBD07-EFDE-4D98-B74C-BF46FE785D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F54750-25A0-4AC2-B494-57AE559C2741}"/>
   <bookViews>
     <workbookView xWindow="-17388" yWindow="-2772" windowWidth="17496" windowHeight="30336" xr2:uid="{4C6B9C08-2C52-4BF9-A6A3-B1CFF437FEB5}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +428,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -752,8 +758,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1928,7 +1934,7 @@
       <c r="B82" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D82">
@@ -1950,10 +1956,10 @@
       <c r="A84" s="19">
         <v>2</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D84">
@@ -1973,7 +1979,7 @@
       <c r="B85" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D85">
@@ -1993,7 +1999,7 @@
       <c r="B86" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D86">
@@ -2010,10 +2016,10 @@
       <c r="A87" s="19">
         <v>5</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="18" t="s">
+      <c r="C87" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D87">
@@ -2030,10 +2036,10 @@
       <c r="A88" s="19">
         <v>6</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D88">
@@ -2050,10 +2056,10 @@
       <c r="A89" s="19">
         <v>7</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C89" s="18" t="s">
+      <c r="C89" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D89">
@@ -2086,7 +2092,7 @@
       <c r="A93" s="18">
         <v>1</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C93" s="18" t="s">
@@ -2109,7 +2115,7 @@
       <c r="B94" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D94">
@@ -2126,10 +2132,10 @@
       <c r="A95" s="18">
         <v>3</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C95" s="18" t="s">
+      <c r="C95" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D95">
@@ -2146,7 +2152,7 @@
       <c r="A96" s="18">
         <v>4</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C96" s="20" t="s">

</xml_diff>